<commit_message>
Changes processing, tables in analysis
</commit_message>
<xml_diff>
--- a/personality and race-IAT study/data/processed/data_processed_codebook.xlsx
+++ b/personality and race-IAT study/data/processed/data_processed_codebook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -47,6 +47,9 @@
     <t xml:space="preserve">exclude_iat_msseconds</t>
   </si>
   <si>
+    <t xml:space="preserve">exclude_iat_accuracy</t>
+  </si>
+  <si>
     <t xml:space="preserve">mean_bfi_a</t>
   </si>
   <si>
@@ -62,13 +65,13 @@
     <t xml:space="preserve">mean_bfi_o</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_a1</t>
+    <t xml:space="preserve">bfi_a1_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_a2</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_a3</t>
+    <t xml:space="preserve">bfi_a3_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_a4</t>
@@ -77,13 +80,13 @@
     <t xml:space="preserve">bfi_a5</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_a6</t>
+    <t xml:space="preserve">bfi_a6_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_a7</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_a8</t>
+    <t xml:space="preserve">bfi_a8_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_a9</t>
@@ -92,16 +95,16 @@
     <t xml:space="preserve">bfi_c1</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_c2</t>
+    <t xml:space="preserve">bfi_c2_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_c3</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_c4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c5</t>
+    <t xml:space="preserve">bfi_c4_recode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c5_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_c6</t>
@@ -113,13 +116,13 @@
     <t xml:space="preserve">bfi_c8</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_c9</t>
+    <t xml:space="preserve">bfi_c9_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_e1</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_e2</t>
+    <t xml:space="preserve">bfi_e2_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_e3</t>
@@ -128,22 +131,52 @@
     <t xml:space="preserve">bfi_e4</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_e5</t>
+    <t xml:space="preserve">bfi_e5_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_e6</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_e7</t>
+    <t xml:space="preserve">bfi_e7_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_e8</t>
   </si>
   <si>
+    <t xml:space="preserve">bfi_o1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o7_recode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o9_recode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o10</t>
+  </si>
+  <si>
     <t xml:space="preserve">bfi_n1</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_n2</t>
+    <t xml:space="preserve">bfi_n2_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_n3</t>
@@ -152,94 +185,16 @@
     <t xml:space="preserve">bfi_n4</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_n5</t>
+    <t xml:space="preserve">bfi_n5_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_n6</t>
   </si>
   <si>
-    <t xml:space="preserve">bfi_n7</t>
+    <t xml:space="preserve">bfi_n7_recode</t>
   </si>
   <si>
     <t xml:space="preserve">bfi_n8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_e2_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_e5_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_e7_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c2_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c4_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c5_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c9_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_n2_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_n5_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_n7_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_a1_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_a3_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_a6_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_a8_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o7_recode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_o9_recode</t>
   </si>
   <si>
     <t xml:space="preserve">age</t>
@@ -960,96 +915,6 @@
       </c>
       <c r="B63"/>
     </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64"/>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65"/>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>66</v>
-      </c>
-      <c r="B66"/>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67"/>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68"/>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69"/>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70"/>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71"/>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
-        <v>72</v>
-      </c>
-      <c r="B72"/>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>73</v>
-      </c>
-      <c r="B73"/>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>74</v>
-      </c>
-      <c r="B74"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>75</v>
-      </c>
-      <c r="B75"/>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>76</v>
-      </c>
-      <c r="B76"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>77</v>
-      </c>
-      <c r="B77"/>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
-        <v>78</v>
-      </c>
-      <c r="B78"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>